<commit_message>
added inventory options by Eblanco
</commit_message>
<xml_diff>
--- a/DBs/Inventario.xlsx
+++ b/DBs/Inventario.xlsx
@@ -20,7 +20,6 @@
   <fonts count="4">
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -67,11 +66,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -153,13 +151,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D1" headerRowCount="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C1" headerRowCount="1">
   <autoFilter ref="A1:B1"/>
-  <tableColumns count="4">
+  <tableColumns count="3">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Nombre"/>
-    <tableColumn id="4" name="Empresa"/>
-    <tableColumn id="5" name="Cantidad"/>
+    <tableColumn id="3" name="Empresa"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -454,13 +451,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="inlineStr">
@@ -478,13 +475,75 @@
           <t>Empresa</t>
         </is>
       </c>
-      <c r="D1" s="0" t="inlineStr">
-        <is>
-          <t>Cantidad</t>
-        </is>
-      </c>
     </row>
-    <row r="1048576" ht="12.8" customHeight="1" s="1"/>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2530</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CLK</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2531</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Monitor</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CLK</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2532</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Mouse</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CLK</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2533</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>xd</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CLK</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
everything is working as expected
</commit_message>
<xml_diff>
--- a/DBs/Inventario.xlsx
+++ b/DBs/Inventario.xlsx
@@ -151,12 +151,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C1" headerRowCount="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D1" headerRowCount="1">
   <autoFilter ref="A1:B1"/>
-  <tableColumns count="3">
+  <tableColumns count="4">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Nombre"/>
-    <tableColumn id="3" name="Empresa"/>
+    <tableColumn id="3" name="Cantidad"/>
+    <tableColumn id="4" name="Fecha de compra"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -451,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -472,75 +473,34 @@
       </c>
       <c r="C1" s="0" t="inlineStr">
         <is>
-          <t>Empresa</t>
+          <t>Cantidad</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>Fecha de compra</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2530</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Laptop</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CLK</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2531</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Monitor</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>CLK</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2532</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Mouse</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>CLK</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2533</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>xd</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>CLK</t>
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>3880</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>Miguel</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>23/12/2023</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Everything is working, we just need to add random IDs to the items in inventory
</commit_message>
<xml_diff>
--- a/DBs/Inventario.xlsx
+++ b/DBs/Inventario.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -482,28 +482,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0" t="inlineStr">
-        <is>
-          <t>3880</t>
-        </is>
-      </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>Miguel</t>
-        </is>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="D2" s="0" t="inlineStr">
-        <is>
-          <t>23/12/2023</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>